<commit_message>
Shorewise 5, AM changes
</commit_message>
<xml_diff>
--- a/setup/column_data_types.xlsx
+++ b/setup/column_data_types.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Isdsf00d03\MentalHealth5\CAPTND\CAPTND_shorewise\scripts\charlie\CAPTND\setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E99DC8F3-66F2-41FA-9FB3-40E1FD0E7135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E2E958-3113-45DF-9031-D846DB2BBBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42630" yWindow="1200" windowWidth="9600" windowHeight="4905" xr2:uid="{85A1D1C1-596B-4787-8657-B7D3C0F7405C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{85A1D1C1-596B-4787-8657-B7D3C0F7405C}"/>
   </bookViews>
   <sheets>
-    <sheet name="SWIFT Subs" sheetId="1" r:id="rId1"/>
+    <sheet name="SWIFT_subs" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
   <si>
     <t>file_id</t>
   </si>
@@ -192,14 +192,28 @@
   </si>
   <si>
     <t>numeric</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -227,8 +241,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,341 +557,420 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9181115-1D87-4AA0-A161-C7983A5DF85C}">
-  <dimension ref="A1:AW2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F854539C-74B0-4F5D-8A29-65927BE3A33E}">
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" customWidth="1"/>
-    <col min="13" max="13" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="36" max="38" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="40" max="42" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="B28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="B31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="B33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="B36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="B37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="B40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="B41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="B42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="B43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="B45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="B46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" t="s">
-        <v>51</v>
-      </c>
-      <c r="O2" t="s">
-        <v>51</v>
-      </c>
-      <c r="P2" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>50</v>
-      </c>
-      <c r="R2" t="s">
-        <v>51</v>
-      </c>
-      <c r="S2" t="s">
-        <v>51</v>
-      </c>
-      <c r="T2" t="s">
-        <v>50</v>
-      </c>
-      <c r="U2" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" t="s">
-        <v>51</v>
-      </c>
-      <c r="W2" t="s">
-        <v>50</v>
-      </c>
-      <c r="X2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AW2" t="s">
+      <c r="B50" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created control script folder, made sure loaddate and file_id are in globalscape data, attempt at postcode validation.
</commit_message>
<xml_diff>
--- a/setup/column_data_types.xlsx
+++ b/setup/column_data_types.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Isdsf00d03\MentalHealth5\CAPTND\CAPTND_shorewise\scripts\charlie\CAPTND\setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E2E958-3113-45DF-9031-D846DB2BBBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29F430B-E1DC-4018-BAD3-AC00B780EC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{85A1D1C1-596B-4787-8657-B7D3C0F7405C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{85A1D1C1-596B-4787-8657-B7D3C0F7405C}"/>
   </bookViews>
   <sheets>
     <sheet name="SWIFT_subs" sheetId="2" r:id="rId1"/>
+    <sheet name="GLOB_subs" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">GLOB_subs!$A$1:$B$47</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="60">
   <si>
     <t>file_id</t>
   </si>
@@ -198,6 +202,24 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>sub_source</t>
+  </si>
+  <si>
+    <t>ref_rej_act</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>In OG Glob</t>
+  </si>
+  <si>
+    <t>loaddate</t>
+  </si>
+  <si>
+    <t>fileid</t>
   </si>
 </sst>
 </file>
@@ -560,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F854539C-74B0-4F5D-8A29-65927BE3A33E}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -973,4 +995,559 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308AD17E-585B-4744-92DC-D93CEC3AB3AF}">
+  <dimension ref="A1:C49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B47" xr:uid="{308AD17E-585B-4744-92DC-D93CEC3AB3AF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B47">
+      <sortCondition ref="B2:B47"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
uniformised load date/ header date and filename /file between globalscape and swift (kept swift format)
</commit_message>
<xml_diff>
--- a/setup/column_data_types.xlsx
+++ b/setup/column_data_types.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Isdsf00d03\MentalHealth5\CAPTND\CAPTND_shorewise\scripts\charlie\CAPTND\setup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\isdsf00d03\MentalHealth5\CAPTND\CAPTND_shorewise\scripts\joana\CAPTND\setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29F430B-E1DC-4018-BAD3-AC00B780EC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B901633D-96A0-4BA1-A507-128C31573B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{85A1D1C1-596B-4787-8657-B7D3C0F7405C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="58">
   <si>
     <t>file_id</t>
   </si>
@@ -214,12 +214,6 @@
   </si>
   <si>
     <t>In OG Glob</t>
-  </si>
-  <si>
-    <t>loaddate</t>
-  </si>
-  <si>
-    <t>fileid</t>
   </si>
 </sst>
 </file>
@@ -586,12 +580,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -599,7 +593,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -607,7 +601,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -615,7 +609,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -623,7 +617,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -631,7 +625,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -639,7 +633,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -647,7 +641,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -655,7 +649,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -663,7 +657,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -671,7 +665,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -679,7 +673,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -687,7 +681,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -695,7 +689,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -703,7 +697,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -711,7 +705,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -719,7 +713,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -727,7 +721,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -735,7 +729,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -743,7 +737,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -751,7 +745,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -759,7 +753,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -767,7 +761,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -775,7 +769,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -783,7 +777,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -791,7 +785,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -799,7 +793,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -807,7 +801,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -815,7 +809,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -823,7 +817,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -831,7 +825,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -839,7 +833,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -847,7 +841,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -855,7 +849,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -863,7 +857,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -871,7 +865,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -879,7 +873,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -887,7 +881,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -895,7 +889,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -903,7 +897,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -911,7 +905,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -919,7 +913,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -927,7 +921,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -935,7 +929,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -943,7 +937,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -951,7 +945,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -959,7 +953,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -967,7 +961,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -975,7 +969,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -983,7 +977,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1001,17 +995,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308AD17E-585B-4744-92DC-D93CEC3AB3AF}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.90625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -1022,7 +1016,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1033,7 +1027,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1044,7 +1038,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1055,7 +1049,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1066,7 +1060,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1077,7 +1071,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1088,7 +1082,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1099,7 +1093,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1110,7 +1104,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1121,7 +1115,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1132,7 +1126,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1143,7 +1137,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1154,7 +1148,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1165,7 +1159,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1176,7 +1170,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1187,7 +1181,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1198,7 +1192,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1209,7 +1203,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1220,7 +1214,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1231,7 +1225,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1242,7 +1236,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1253,7 +1247,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1264,7 +1258,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1275,7 +1269,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1286,7 +1280,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1297,7 +1291,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1308,7 +1302,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1319,7 +1313,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1330,7 +1324,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1341,7 +1335,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1352,7 +1346,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1363,7 +1357,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1374,7 +1368,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1385,7 +1379,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1396,7 +1390,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1407,7 +1401,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1418,7 +1412,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1429,7 +1423,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1440,7 +1434,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -1451,7 +1445,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -1462,7 +1456,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -1473,7 +1467,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -1484,7 +1478,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -1495,7 +1489,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -1506,7 +1500,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1517,7 +1511,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1528,17 +1522,20 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B48" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>